<commit_message>
HighUsers.json SiteUsageByBlockLevel.json files data modified.
</commit_message>
<xml_diff>
--- a/DB/sample/TreeMap-SiteUsageByBlockLevel.xlsx
+++ b/DB/sample/TreeMap-SiteUsageByBlockLevel.xlsx
@@ -1,25 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F10FAA2-84E9-4430-8536-83BE061E1CFE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Request" sheetId="1" r:id="rId1"/>
     <sheet name="Block Details" sheetId="2" r:id="rId2"/>
     <sheet name="House Details" sheetId="3" r:id="rId3"/>
     <sheet name="Day Usage for House" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet4" sheetId="5" r:id="rId5"/>
+    <sheet name="Resonse" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="719">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="720">
   <si>
     <t>uid</t>
   </si>
@@ -2176,12 +2175,15 @@
   </si>
   <si>
     <t>12W001</t>
+  </si>
+  <si>
+    <t>value</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2226,7 +2228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2239,6 +2241,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2332,23 +2335,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2384,23 +2370,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2576,7 +2545,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2627,11 +2596,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2983,11 +2952,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:BH70"/>
   <sheetViews>
     <sheetView topLeftCell="AJ1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:BH7"/>
+      <selection activeCell="AR10" sqref="AR10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11657,97 +11626,97 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B2:BH6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:BT6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:60" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:72" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>26</v>
       </c>
       <c r="C2">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>26</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>6</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>26</v>
       </c>
-      <c r="M2">
+      <c r="O2">
         <v>7</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="T2" t="s">
         <v>26</v>
       </c>
-      <c r="R2">
+      <c r="U2">
         <v>8</v>
       </c>
-      <c r="V2" t="s">
+      <c r="Z2" t="s">
         <v>26</v>
       </c>
-      <c r="W2">
+      <c r="AA2">
         <v>9</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB2">
-        <v>10</v>
       </c>
       <c r="AF2" t="s">
         <v>26</v>
       </c>
       <c r="AG2">
+        <v>10</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AM2">
         <v>11</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AR2" t="s">
         <v>26</v>
       </c>
-      <c r="AL2">
+      <c r="AS2">
         <v>12</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AX2" t="s">
         <v>26</v>
       </c>
-      <c r="AQ2">
+      <c r="AY2">
         <v>13</v>
       </c>
-      <c r="AU2" t="s">
+      <c r="BD2" t="s">
         <v>26</v>
       </c>
-      <c r="AV2">
+      <c r="BE2">
         <v>14</v>
       </c>
-      <c r="AZ2" t="s">
+      <c r="BJ2" t="s">
         <v>26</v>
       </c>
-      <c r="BA2">
+      <c r="BK2">
         <v>15</v>
       </c>
-      <c r="BE2" t="s">
+      <c r="BP2" t="s">
         <v>26</v>
       </c>
-      <c r="BF2">
+      <c r="BQ2">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="2:60" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:72" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
@@ -11760,65 +11729,68 @@
       <c r="E3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="F3" s="6" t="s">
+        <v>719</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="J3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="K3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="6" t="s">
+        <v>719</v>
+      </c>
+      <c r="N3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="O3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="P3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="Q3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="R3" s="6" t="s">
+        <v>719</v>
+      </c>
+      <c r="T3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="4" t="s">
+      <c r="U3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="S3" s="4" t="s">
+      <c r="V3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="T3" s="4" t="s">
+      <c r="W3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="V3" s="4" t="s">
+      <c r="X3" s="6" t="s">
+        <v>719</v>
+      </c>
+      <c r="Z3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="W3" s="4" t="s">
+      <c r="AA3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="X3" s="4" t="s">
+      <c r="AB3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="Y3" s="4" t="s">
+      <c r="AC3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AA3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="AB3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="AC3" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD3" s="4" t="s">
-        <v>28</v>
+      <c r="AD3" s="6" t="s">
+        <v>719</v>
       </c>
       <c r="AF3" s="4" t="s">
         <v>6</v>
@@ -11832,68 +11804,101 @@
       <c r="AI3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AK3" s="4" t="s">
+      <c r="AJ3" s="6" t="s">
+        <v>719</v>
+      </c>
+      <c r="AL3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="AL3" s="4" t="s">
+      <c r="AM3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AM3" s="4" t="s">
+      <c r="AN3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AN3" s="4" t="s">
+      <c r="AO3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AP3" s="4" t="s">
+      <c r="AP3" s="6" t="s">
+        <v>719</v>
+      </c>
+      <c r="AR3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="AQ3" s="4" t="s">
+      <c r="AS3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AR3" s="4" t="s">
+      <c r="AT3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AS3" s="4" t="s">
+      <c r="AU3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AU3" s="4" t="s">
+      <c r="AV3" s="6" t="s">
+        <v>719</v>
+      </c>
+      <c r="AX3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="AV3" s="4" t="s">
+      <c r="AY3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AW3" s="4" t="s">
+      <c r="AZ3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AX3" s="4" t="s">
+      <c r="BA3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AZ3" s="4" t="s">
+      <c r="BB3" s="6" t="s">
+        <v>719</v>
+      </c>
+      <c r="BD3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="BA3" s="4" t="s">
+      <c r="BE3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="BB3" s="4" t="s">
+      <c r="BF3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="BC3" s="4" t="s">
+      <c r="BG3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="BE3" s="4" t="s">
+      <c r="BH3" s="6" t="s">
+        <v>719</v>
+      </c>
+      <c r="BJ3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="BF3" s="4" t="s">
+      <c r="BK3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="BG3" s="4" t="s">
+      <c r="BL3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="BH3" s="4" t="s">
+      <c r="BM3" s="4" t="s">
         <v>28</v>
       </c>
+      <c r="BN3" s="6" t="s">
+        <v>719</v>
+      </c>
+      <c r="BP3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="BQ3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="BR3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="BS3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="BT3" s="6" t="s">
+        <v>719</v>
+      </c>
     </row>
-    <row r="4" spans="2:60" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:72" x14ac:dyDescent="0.25">
       <c r="B4" s="4">
         <v>1</v>
       </c>
@@ -11906,140 +11911,176 @@
       <c r="E4" s="4">
         <v>5</v>
       </c>
-      <c r="G4" s="4">
+      <c r="F4" s="5">
+        <v>27414</v>
+      </c>
+      <c r="H4" s="4">
         <v>1</v>
       </c>
-      <c r="H4" s="4">
+      <c r="I4" s="4">
         <v>77</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="J4" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="J4" s="4">
+      <c r="K4" s="4">
         <v>6</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4" s="5">
+        <v>2386</v>
+      </c>
+      <c r="N4" s="4">
         <v>1</v>
       </c>
-      <c r="M4" s="4">
+      <c r="O4" s="4">
         <v>208</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="P4" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="O4" s="4">
+      <c r="Q4" s="4">
         <v>7</v>
       </c>
-      <c r="Q4" s="4">
+      <c r="R4" s="5">
+        <v>10796</v>
+      </c>
+      <c r="T4" s="4">
         <v>1</v>
       </c>
-      <c r="R4" s="4">
+      <c r="U4" s="4">
         <v>269</v>
       </c>
-      <c r="S4" s="4" t="s">
+      <c r="V4" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="T4" s="4">
+      <c r="W4" s="4">
         <v>8</v>
       </c>
-      <c r="V4" s="4">
+      <c r="X4" s="4">
+        <v>5</v>
+      </c>
+      <c r="Z4" s="4">
         <v>1</v>
       </c>
-      <c r="W4" s="4">
+      <c r="AA4" s="4">
         <v>332</v>
       </c>
-      <c r="X4" s="4" t="s">
+      <c r="AB4" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="Y4" s="4">
+      <c r="AC4" s="4">
         <v>9</v>
       </c>
-      <c r="AA4" s="4">
-        <v>1</v>
-      </c>
-      <c r="AB4" s="4">
-        <v>397</v>
-      </c>
-      <c r="AC4" s="4" t="s">
-        <v>315</v>
-      </c>
-      <c r="AD4" s="4">
-        <v>10</v>
+      <c r="AD4" s="5">
+        <v>3171</v>
       </c>
       <c r="AF4" s="4">
         <v>1</v>
       </c>
       <c r="AG4" s="4">
+        <v>397</v>
+      </c>
+      <c r="AH4" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="AI4" s="4">
+        <v>10</v>
+      </c>
+      <c r="AJ4" s="4">
+        <v>370</v>
+      </c>
+      <c r="AL4" s="4">
+        <v>1</v>
+      </c>
+      <c r="AM4" s="4">
         <v>459</v>
       </c>
-      <c r="AH4" s="4" t="s">
+      <c r="AN4" s="4" t="s">
         <v>378</v>
       </c>
-      <c r="AI4" s="4">
+      <c r="AO4" s="4">
         <v>11</v>
       </c>
-      <c r="AK4" s="4">
+      <c r="AP4" s="5">
+        <v>6581</v>
+      </c>
+      <c r="AR4" s="4">
         <v>1</v>
       </c>
-      <c r="AL4" s="4">
+      <c r="AS4" s="4">
         <v>509</v>
       </c>
-      <c r="AM4" s="4" t="s">
+      <c r="AT4" s="4" t="s">
         <v>426</v>
       </c>
-      <c r="AN4" s="4">
+      <c r="AU4" s="4">
         <v>12</v>
       </c>
-      <c r="AP4" s="4">
+      <c r="AV4" s="5">
+        <v>12273</v>
+      </c>
+      <c r="AX4" s="4">
         <v>1</v>
       </c>
-      <c r="AQ4" s="4">
+      <c r="AY4" s="4">
         <v>553</v>
       </c>
-      <c r="AR4" s="4" t="s">
+      <c r="AZ4" s="4" t="s">
         <v>471</v>
       </c>
-      <c r="AS4" s="4">
+      <c r="BA4" s="4">
         <v>13</v>
       </c>
-      <c r="AU4" s="4">
+      <c r="BB4" s="4">
+        <v>2</v>
+      </c>
+      <c r="BD4" s="4">
         <v>1</v>
       </c>
-      <c r="AV4" s="4">
+      <c r="BE4" s="4">
         <v>614</v>
       </c>
-      <c r="AW4" s="4" t="s">
+      <c r="BF4" s="4" t="s">
         <v>533</v>
       </c>
-      <c r="AX4" s="4">
+      <c r="BG4" s="4">
         <v>14</v>
       </c>
-      <c r="AZ4" s="4">
+      <c r="BH4" s="4">
+        <v>477</v>
+      </c>
+      <c r="BJ4" s="4">
         <v>1</v>
       </c>
-      <c r="BA4" s="4">
+      <c r="BK4" s="4">
         <v>675</v>
       </c>
-      <c r="BB4" s="4" t="s">
+      <c r="BL4" s="4" t="s">
         <v>595</v>
       </c>
-      <c r="BC4" s="4">
+      <c r="BM4" s="4">
         <v>15</v>
       </c>
-      <c r="BE4" s="4">
+      <c r="BN4" s="5">
+        <v>2456</v>
+      </c>
+      <c r="BP4" s="4">
         <v>1</v>
       </c>
-      <c r="BF4" s="4">
+      <c r="BQ4" s="4">
         <v>736</v>
       </c>
-      <c r="BG4" s="4" t="s">
+      <c r="BR4" s="4" t="s">
         <v>657</v>
       </c>
-      <c r="BH4" s="4">
+      <c r="BS4" s="4">
         <v>16</v>
       </c>
+      <c r="BT4" s="5">
+        <v>5923</v>
+      </c>
     </row>
-    <row r="5" spans="2:60" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:72" x14ac:dyDescent="0.25">
       <c r="B5" s="4">
         <v>2</v>
       </c>
@@ -12052,140 +12093,176 @@
       <c r="E5" s="4">
         <v>5</v>
       </c>
-      <c r="G5" s="4">
+      <c r="F5" s="5">
+        <v>42518</v>
+      </c>
+      <c r="H5" s="4">
         <v>2</v>
       </c>
-      <c r="H5" s="4">
+      <c r="I5" s="4">
         <v>78</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="J5" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="J5" s="4">
+      <c r="K5" s="4">
         <v>6</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5" s="6">
+        <v>130</v>
+      </c>
+      <c r="N5" s="4">
         <v>2</v>
       </c>
-      <c r="M5" s="4">
+      <c r="O5" s="4">
         <v>209</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="P5" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="O5" s="4">
+      <c r="Q5" s="4">
         <v>7</v>
       </c>
-      <c r="Q5" s="4">
+      <c r="R5" s="5">
+        <v>9709</v>
+      </c>
+      <c r="T5" s="4">
         <v>2</v>
       </c>
-      <c r="R5" s="4">
+      <c r="U5" s="4">
         <v>270</v>
       </c>
-      <c r="S5" s="4" t="s">
+      <c r="V5" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="T5" s="4">
+      <c r="W5" s="4">
         <v>8</v>
       </c>
-      <c r="V5" s="4">
+      <c r="X5" s="5">
+        <v>5883</v>
+      </c>
+      <c r="Z5" s="4">
         <v>2</v>
       </c>
-      <c r="W5" s="4">
+      <c r="AA5" s="4">
         <v>333</v>
       </c>
-      <c r="X5" s="4" t="s">
+      <c r="AB5" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="Y5" s="4">
+      <c r="AC5" s="4">
         <v>9</v>
       </c>
-      <c r="AA5" s="4">
-        <v>2</v>
-      </c>
-      <c r="AB5" s="4">
-        <v>398</v>
-      </c>
-      <c r="AC5" s="4" t="s">
-        <v>316</v>
-      </c>
-      <c r="AD5" s="4">
-        <v>10</v>
+      <c r="AD5" s="5">
+        <v>9087</v>
       </c>
       <c r="AF5" s="4">
         <v>2</v>
       </c>
       <c r="AG5" s="4">
+        <v>398</v>
+      </c>
+      <c r="AH5" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="AI5" s="4">
+        <v>10</v>
+      </c>
+      <c r="AJ5" s="5">
+        <v>5063</v>
+      </c>
+      <c r="AL5" s="4">
+        <v>2</v>
+      </c>
+      <c r="AM5" s="4">
         <v>460</v>
       </c>
-      <c r="AH5" s="4" t="s">
+      <c r="AN5" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="AI5" s="4">
+      <c r="AO5" s="4">
         <v>11</v>
       </c>
-      <c r="AK5" s="4">
+      <c r="AP5" s="5">
+        <v>3394</v>
+      </c>
+      <c r="AR5" s="4">
         <v>2</v>
       </c>
-      <c r="AL5" s="4">
+      <c r="AS5" s="4">
         <v>510</v>
       </c>
-      <c r="AM5" s="4" t="s">
+      <c r="AT5" s="4" t="s">
         <v>427</v>
       </c>
-      <c r="AN5" s="4">
+      <c r="AU5" s="4">
         <v>12</v>
       </c>
-      <c r="AP5" s="4">
+      <c r="AV5" s="5">
+        <v>2066</v>
+      </c>
+      <c r="AX5" s="4">
         <v>2</v>
       </c>
-      <c r="AQ5" s="4">
+      <c r="AY5" s="4">
         <v>554</v>
       </c>
-      <c r="AR5" s="4" t="s">
+      <c r="AZ5" s="4" t="s">
         <v>472</v>
       </c>
-      <c r="AS5" s="4">
+      <c r="BA5" s="4">
         <v>13</v>
       </c>
-      <c r="AU5" s="4">
+      <c r="BB5" s="5">
+        <v>8635</v>
+      </c>
+      <c r="BD5" s="4">
         <v>2</v>
       </c>
-      <c r="AV5" s="4">
+      <c r="BE5" s="4">
         <v>615</v>
       </c>
-      <c r="AW5" s="4" t="s">
+      <c r="BF5" s="4" t="s">
         <v>534</v>
       </c>
-      <c r="AX5" s="4">
+      <c r="BG5" s="4">
         <v>14</v>
       </c>
-      <c r="AZ5" s="4">
+      <c r="BH5" s="5">
+        <v>2011</v>
+      </c>
+      <c r="BJ5" s="4">
         <v>2</v>
       </c>
-      <c r="BA5" s="4">
+      <c r="BK5" s="4">
         <v>676</v>
       </c>
-      <c r="BB5" s="4" t="s">
+      <c r="BL5" s="4" t="s">
         <v>596</v>
       </c>
-      <c r="BC5" s="4">
+      <c r="BM5" s="4">
         <v>15</v>
       </c>
-      <c r="BE5" s="4">
+      <c r="BN5" s="5">
+        <v>12911</v>
+      </c>
+      <c r="BP5" s="4">
         <v>2</v>
       </c>
-      <c r="BF5" s="4">
+      <c r="BQ5" s="4">
         <v>737</v>
       </c>
-      <c r="BG5" s="4" t="s">
+      <c r="BR5" s="4" t="s">
         <v>658</v>
       </c>
-      <c r="BH5" s="4">
+      <c r="BS5" s="4">
         <v>16</v>
       </c>
+      <c r="BT5" s="5">
+        <v>9173</v>
+      </c>
     </row>
-    <row r="6" spans="2:60" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:72" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
         <v>3</v>
       </c>
@@ -12198,137 +12275,173 @@
       <c r="E6" s="4">
         <v>5</v>
       </c>
-      <c r="G6" s="4">
+      <c r="F6" s="5">
+        <v>27128</v>
+      </c>
+      <c r="H6" s="4">
         <v>3</v>
       </c>
-      <c r="H6" s="4">
+      <c r="I6" s="4">
         <v>79</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="J6" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="J6" s="4">
+      <c r="K6" s="4">
         <v>6</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L6" s="5">
+        <v>1692</v>
+      </c>
+      <c r="N6" s="4">
         <v>3</v>
       </c>
-      <c r="M6" s="4">
+      <c r="O6" s="4">
         <v>210</v>
       </c>
-      <c r="N6" s="4" t="s">
+      <c r="P6" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="O6" s="4">
+      <c r="Q6" s="4">
         <v>7</v>
       </c>
-      <c r="Q6" s="4">
+      <c r="R6" s="5">
+        <v>11676</v>
+      </c>
+      <c r="T6" s="4">
         <v>3</v>
       </c>
-      <c r="R6" s="4">
+      <c r="U6" s="4">
         <v>271</v>
       </c>
-      <c r="S6" s="4" t="s">
+      <c r="V6" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="T6" s="4">
+      <c r="W6" s="4">
         <v>8</v>
       </c>
-      <c r="V6" s="4">
+      <c r="X6" s="5">
+        <v>11588</v>
+      </c>
+      <c r="Z6" s="4">
         <v>3</v>
       </c>
-      <c r="W6" s="4">
+      <c r="AA6" s="4">
         <v>334</v>
       </c>
-      <c r="X6" s="4" t="s">
+      <c r="AB6" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="Y6" s="4">
+      <c r="AC6" s="4">
         <v>9</v>
       </c>
-      <c r="AA6" s="4">
-        <v>3</v>
-      </c>
-      <c r="AB6" s="4">
-        <v>399</v>
-      </c>
-      <c r="AC6" s="4" t="s">
-        <v>317</v>
-      </c>
-      <c r="AD6" s="4">
-        <v>10</v>
+      <c r="AD6" s="5">
+        <v>2569</v>
       </c>
       <c r="AF6" s="4">
         <v>3</v>
       </c>
       <c r="AG6" s="4">
+        <v>399</v>
+      </c>
+      <c r="AH6" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="AI6" s="4">
+        <v>10</v>
+      </c>
+      <c r="AJ6" s="5">
+        <v>4490</v>
+      </c>
+      <c r="AL6" s="4">
+        <v>3</v>
+      </c>
+      <c r="AM6" s="4">
         <v>461</v>
       </c>
-      <c r="AH6" s="4" t="s">
+      <c r="AN6" s="4" t="s">
         <v>380</v>
       </c>
-      <c r="AI6" s="4">
+      <c r="AO6" s="4">
         <v>11</v>
       </c>
-      <c r="AK6" s="4">
+      <c r="AP6" s="5">
+        <v>4640</v>
+      </c>
+      <c r="AR6" s="4">
         <v>3</v>
       </c>
-      <c r="AL6" s="4">
+      <c r="AS6" s="4">
         <v>511</v>
       </c>
-      <c r="AM6" s="4" t="s">
+      <c r="AT6" s="4" t="s">
         <v>428</v>
       </c>
-      <c r="AN6" s="4">
+      <c r="AU6" s="4">
         <v>12</v>
       </c>
-      <c r="AP6" s="4">
+      <c r="AV6" s="5">
+        <v>3686</v>
+      </c>
+      <c r="AX6" s="4">
         <v>3</v>
       </c>
-      <c r="AQ6" s="4">
+      <c r="AY6" s="4">
         <v>555</v>
       </c>
-      <c r="AR6" s="4" t="s">
+      <c r="AZ6" s="4" t="s">
         <v>473</v>
       </c>
-      <c r="AS6" s="4">
+      <c r="BA6" s="4">
         <v>13</v>
       </c>
-      <c r="AU6" s="4">
+      <c r="BB6" s="4">
+        <v>0</v>
+      </c>
+      <c r="BD6" s="4">
         <v>3</v>
       </c>
-      <c r="AV6" s="4">
+      <c r="BE6" s="4">
         <v>616</v>
       </c>
-      <c r="AW6" s="4" t="s">
+      <c r="BF6" s="4" t="s">
         <v>535</v>
       </c>
-      <c r="AX6" s="4">
+      <c r="BG6" s="4">
         <v>14</v>
       </c>
-      <c r="AZ6" s="4">
+      <c r="BH6" s="5">
+        <v>1311</v>
+      </c>
+      <c r="BJ6" s="4">
         <v>3</v>
       </c>
-      <c r="BA6" s="4">
+      <c r="BK6" s="4">
         <v>677</v>
       </c>
-      <c r="BB6" s="4" t="s">
+      <c r="BL6" s="4" t="s">
         <v>597</v>
       </c>
-      <c r="BC6" s="4">
+      <c r="BM6" s="4">
         <v>15</v>
       </c>
-      <c r="BE6" s="4">
+      <c r="BN6" s="5">
+        <v>517</v>
+      </c>
+      <c r="BP6" s="4">
         <v>3</v>
       </c>
-      <c r="BF6" s="4">
+      <c r="BQ6" s="4">
         <v>738</v>
       </c>
-      <c r="BG6" s="4" t="s">
+      <c r="BR6" s="4" t="s">
         <v>659</v>
       </c>
-      <c r="BH6" s="4">
+      <c r="BS6" s="4">
         <v>16</v>
+      </c>
+      <c r="BT6" s="5">
+        <v>4694</v>
       </c>
     </row>
   </sheetData>
@@ -12337,7 +12450,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>